<commit_message>
Uploading Project Plan Gantt Chart
</commit_message>
<xml_diff>
--- a/Documentation/Agile-Project-Plan.xlsx
+++ b/Documentation/Agile-Project-Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4cff5697cfe4737/University/Year 4 (Masters) - 1st Year/Semester B/CMP9134M - Advanced Software Engineering/Assessment 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="13_ncr:1_{5637A24D-25EC-4458-9528-639E6615948E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4E6812F-9D13-4C12-84E3-45EAAF3BB8D4}"/>
+  <xr:revisionPtr revIDLastSave="366" documentId="13_ncr:1_{5637A24D-25EC-4458-9528-639E6615948E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEC89452-3472-445D-A0BA-CCEBBBEDEAE4}"/>
   <bookViews>
-    <workbookView xWindow="25520" yWindow="-7160" windowWidth="38560" windowHeight="21040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-7290" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="3" r:id="rId1"/>
@@ -1198,6 +1198,27 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1216,13 +1237,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1232,39 +1265,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1298,6 +1298,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1494,9 +1498,9 @@
   </sheetPr>
   <dimension ref="B1:CE33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
+      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1566,7 +1570,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="54">
-        <v>45329</v>
+        <v>45322</v>
       </c>
     </row>
     <row r="6" spans="2:83" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1580,89 +1584,89 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="85"/>
-      <c r="S7" s="85"/>
-      <c r="T7" s="85"/>
-      <c r="U7" s="85"/>
-      <c r="V7" s="85"/>
-      <c r="W7" s="85"/>
-      <c r="X7" s="85"/>
-      <c r="Y7" s="85"/>
-      <c r="Z7" s="85"/>
-      <c r="AA7" s="85"/>
-      <c r="AB7" s="86"/>
-      <c r="AC7" s="78" t="s">
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="83"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="84"/>
+      <c r="AC7" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="AD7" s="79"/>
-      <c r="AE7" s="79"/>
-      <c r="AF7" s="79"/>
-      <c r="AG7" s="79"/>
-      <c r="AH7" s="79"/>
-      <c r="AI7" s="79"/>
-      <c r="AJ7" s="79"/>
-      <c r="AK7" s="79"/>
-      <c r="AL7" s="79"/>
-      <c r="AM7" s="79"/>
-      <c r="AN7" s="79"/>
-      <c r="AO7" s="79"/>
-      <c r="AP7" s="79"/>
-      <c r="AQ7" s="79"/>
-      <c r="AR7" s="79"/>
-      <c r="AS7" s="79"/>
-      <c r="AT7" s="79"/>
-      <c r="AU7" s="79"/>
-      <c r="AV7" s="80"/>
-      <c r="AW7" s="81" t="s">
+      <c r="AD7" s="86"/>
+      <c r="AE7" s="86"/>
+      <c r="AF7" s="86"/>
+      <c r="AG7" s="86"/>
+      <c r="AH7" s="86"/>
+      <c r="AI7" s="86"/>
+      <c r="AJ7" s="86"/>
+      <c r="AK7" s="86"/>
+      <c r="AL7" s="86"/>
+      <c r="AM7" s="86"/>
+      <c r="AN7" s="86"/>
+      <c r="AO7" s="86"/>
+      <c r="AP7" s="86"/>
+      <c r="AQ7" s="86"/>
+      <c r="AR7" s="86"/>
+      <c r="AS7" s="86"/>
+      <c r="AT7" s="86"/>
+      <c r="AU7" s="86"/>
+      <c r="AV7" s="87"/>
+      <c r="AW7" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="AX7" s="82"/>
-      <c r="AY7" s="82"/>
-      <c r="AZ7" s="82"/>
-      <c r="BA7" s="82"/>
-      <c r="BB7" s="82"/>
-      <c r="BC7" s="82"/>
-      <c r="BD7" s="82"/>
-      <c r="BE7" s="82"/>
-      <c r="BF7" s="82"/>
-      <c r="BG7" s="82"/>
-      <c r="BH7" s="82"/>
-      <c r="BI7" s="82"/>
-      <c r="BJ7" s="82"/>
-      <c r="BK7" s="82"/>
-      <c r="BL7" s="82"/>
-      <c r="BM7" s="82"/>
-      <c r="BN7" s="82"/>
-      <c r="BO7" s="82"/>
-      <c r="BP7" s="83"/>
-      <c r="BQ7" s="98" t="s">
+      <c r="AX7" s="89"/>
+      <c r="AY7" s="89"/>
+      <c r="AZ7" s="89"/>
+      <c r="BA7" s="89"/>
+      <c r="BB7" s="89"/>
+      <c r="BC7" s="89"/>
+      <c r="BD7" s="89"/>
+      <c r="BE7" s="89"/>
+      <c r="BF7" s="89"/>
+      <c r="BG7" s="89"/>
+      <c r="BH7" s="89"/>
+      <c r="BI7" s="89"/>
+      <c r="BJ7" s="89"/>
+      <c r="BK7" s="89"/>
+      <c r="BL7" s="89"/>
+      <c r="BM7" s="89"/>
+      <c r="BN7" s="89"/>
+      <c r="BO7" s="89"/>
+      <c r="BP7" s="90"/>
+      <c r="BQ7" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="BR7" s="99"/>
-      <c r="BS7" s="99"/>
-      <c r="BT7" s="99"/>
-      <c r="BU7" s="99"/>
-      <c r="BV7" s="99"/>
-      <c r="BW7" s="99"/>
-      <c r="BX7" s="99"/>
-      <c r="BY7" s="99"/>
-      <c r="BZ7" s="99"/>
-      <c r="CA7" s="99"/>
-      <c r="CB7" s="99"/>
-      <c r="CC7" s="99"/>
-      <c r="CD7" s="99"/>
-      <c r="CE7" s="100"/>
+      <c r="BR7" s="80"/>
+      <c r="BS7" s="80"/>
+      <c r="BT7" s="80"/>
+      <c r="BU7" s="80"/>
+      <c r="BV7" s="80"/>
+      <c r="BW7" s="80"/>
+      <c r="BX7" s="80"/>
+      <c r="BY7" s="80"/>
+      <c r="BZ7" s="80"/>
+      <c r="CA7" s="80"/>
+      <c r="CB7" s="80"/>
+      <c r="CC7" s="80"/>
+      <c r="CD7" s="80"/>
+      <c r="CE7" s="81"/>
     </row>
     <row r="8" spans="2:83" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
@@ -1686,111 +1690,111 @@
       <c r="H8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="93" t="s">
+      <c r="I8" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="91"/>
-      <c r="N8" s="91" t="s">
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="92"/>
+      <c r="N8" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="O8" s="91"/>
-      <c r="P8" s="91"/>
-      <c r="Q8" s="91"/>
-      <c r="R8" s="91"/>
-      <c r="S8" s="91" t="s">
+      <c r="O8" s="92"/>
+      <c r="P8" s="92"/>
+      <c r="Q8" s="92"/>
+      <c r="R8" s="92"/>
+      <c r="S8" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="T8" s="91"/>
-      <c r="U8" s="91"/>
-      <c r="V8" s="91"/>
-      <c r="W8" s="92"/>
-      <c r="X8" s="91" t="s">
+      <c r="T8" s="92"/>
+      <c r="U8" s="92"/>
+      <c r="V8" s="92"/>
+      <c r="W8" s="93"/>
+      <c r="X8" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="Y8" s="91"/>
-      <c r="Z8" s="91"/>
-      <c r="AA8" s="91"/>
-      <c r="AB8" s="92"/>
-      <c r="AC8" s="95" t="s">
+      <c r="Y8" s="92"/>
+      <c r="Z8" s="92"/>
+      <c r="AA8" s="92"/>
+      <c r="AB8" s="93"/>
+      <c r="AC8" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="AD8" s="96"/>
-      <c r="AE8" s="96"/>
-      <c r="AF8" s="96"/>
-      <c r="AG8" s="96"/>
-      <c r="AH8" s="96" t="s">
+      <c r="AD8" s="95"/>
+      <c r="AE8" s="95"/>
+      <c r="AF8" s="95"/>
+      <c r="AG8" s="95"/>
+      <c r="AH8" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="AI8" s="96"/>
-      <c r="AJ8" s="96"/>
-      <c r="AK8" s="96"/>
-      <c r="AL8" s="96"/>
-      <c r="AM8" s="96" t="s">
+      <c r="AI8" s="95"/>
+      <c r="AJ8" s="95"/>
+      <c r="AK8" s="95"/>
+      <c r="AL8" s="95"/>
+      <c r="AM8" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="AN8" s="96"/>
-      <c r="AO8" s="96"/>
-      <c r="AP8" s="96"/>
-      <c r="AQ8" s="96"/>
-      <c r="AR8" s="96" t="s">
+      <c r="AN8" s="95"/>
+      <c r="AO8" s="95"/>
+      <c r="AP8" s="95"/>
+      <c r="AQ8" s="95"/>
+      <c r="AR8" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="AS8" s="96"/>
-      <c r="AT8" s="96"/>
-      <c r="AU8" s="96"/>
-      <c r="AV8" s="97"/>
-      <c r="AW8" s="94" t="s">
+      <c r="AS8" s="95"/>
+      <c r="AT8" s="95"/>
+      <c r="AU8" s="95"/>
+      <c r="AV8" s="96"/>
+      <c r="AW8" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="AX8" s="87"/>
-      <c r="AY8" s="87"/>
-      <c r="AZ8" s="87"/>
-      <c r="BA8" s="87"/>
-      <c r="BB8" s="87" t="s">
+      <c r="AX8" s="98"/>
+      <c r="AY8" s="98"/>
+      <c r="AZ8" s="98"/>
+      <c r="BA8" s="98"/>
+      <c r="BB8" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="BC8" s="87"/>
-      <c r="BD8" s="87"/>
-      <c r="BE8" s="87"/>
-      <c r="BF8" s="87"/>
-      <c r="BG8" s="87" t="s">
+      <c r="BC8" s="98"/>
+      <c r="BD8" s="98"/>
+      <c r="BE8" s="98"/>
+      <c r="BF8" s="98"/>
+      <c r="BG8" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="BH8" s="87"/>
-      <c r="BI8" s="87"/>
-      <c r="BJ8" s="87"/>
-      <c r="BK8" s="87"/>
-      <c r="BL8" s="87" t="s">
+      <c r="BH8" s="98"/>
+      <c r="BI8" s="98"/>
+      <c r="BJ8" s="98"/>
+      <c r="BK8" s="98"/>
+      <c r="BL8" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="BM8" s="87"/>
-      <c r="BN8" s="87"/>
-      <c r="BO8" s="87"/>
-      <c r="BP8" s="88"/>
-      <c r="BQ8" s="89" t="s">
+      <c r="BM8" s="98"/>
+      <c r="BN8" s="98"/>
+      <c r="BO8" s="98"/>
+      <c r="BP8" s="99"/>
+      <c r="BQ8" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="BR8" s="90"/>
-      <c r="BS8" s="90"/>
-      <c r="BT8" s="90"/>
-      <c r="BU8" s="90"/>
-      <c r="BV8" s="90" t="s">
+      <c r="BR8" s="78"/>
+      <c r="BS8" s="78"/>
+      <c r="BT8" s="78"/>
+      <c r="BU8" s="78"/>
+      <c r="BV8" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="BW8" s="90"/>
-      <c r="BX8" s="90"/>
-      <c r="BY8" s="90"/>
-      <c r="BZ8" s="90"/>
-      <c r="CA8" s="90" t="s">
+      <c r="BW8" s="78"/>
+      <c r="BX8" s="78"/>
+      <c r="BY8" s="78"/>
+      <c r="BZ8" s="78"/>
+      <c r="CA8" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="CB8" s="90"/>
-      <c r="CC8" s="90"/>
-      <c r="CD8" s="90"/>
-      <c r="CE8" s="90"/>
+      <c r="CB8" s="78"/>
+      <c r="CC8" s="78"/>
+      <c r="CD8" s="78"/>
+      <c r="CE8" s="78"/>
     </row>
     <row r="9" spans="2:83" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
@@ -3688,6 +3692,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="S8:W8"/>
+    <mergeCell ref="AM8:AQ8"/>
+    <mergeCell ref="BG8:BK8"/>
     <mergeCell ref="CA8:CE8"/>
     <mergeCell ref="BQ7:CE7"/>
     <mergeCell ref="I7:AB7"/>
@@ -3704,9 +3711,6 @@
     <mergeCell ref="BL8:BP8"/>
     <mergeCell ref="BQ8:BU8"/>
     <mergeCell ref="BV8:BZ8"/>
-    <mergeCell ref="S8:W8"/>
-    <mergeCell ref="AM8:AQ8"/>
-    <mergeCell ref="BG8:BK8"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:H26">
     <cfRule type="dataBar" priority="10">

</xml_diff>